<commit_message>
done the sql commands, and getGottenEggs (also gives next eggs)
</commit_message>
<xml_diff>
--- a/db_plan.xlsx
+++ b/db_plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>EggID</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>userID</t>
-  </si>
-  <si>
-    <t>Egg_FoundID</t>
   </si>
   <si>
     <t>EggID_to</t>
@@ -385,7 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -400,13 +397,13 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -416,33 +413,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -455,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +460,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -482,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +486,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>